<commit_message>
fixed issue with L1 on BoM
</commit_message>
<xml_diff>
--- a/EDA/BoSLcam_bom_rev1.2.0.xlsx
+++ b/EDA/BoSLcam_bom_rev1.2.0.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stephen\Documents\Repositories\BoSLcam\EDA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F46FA51-5287-428A-9C85-FF7F7558E146}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{844AF2E7-00F9-4C3C-8B1C-AC7D18E09B13}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="28920" windowHeight="12495" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -145,12 +145,6 @@
     <t>9.1 nH</t>
   </si>
   <si>
-    <t>https://au.mouser.com/ProductDetail/TDK/MLG0603P9N1HT000/?qs=u4%252BEJ9urDAQc/lR37YK7mA==</t>
-  </si>
-  <si>
-    <t>MLG0603P9N1HT000</t>
-  </si>
-  <si>
     <t>39 Ω</t>
   </si>
   <si>
@@ -416,6 +410,12 @@
   </si>
   <si>
     <t>C2,C3,C5,C8,C11,C18,C19</t>
+  </si>
+  <si>
+    <t>LQW18AN9N1D00D</t>
+  </si>
+  <si>
+    <t>https://au.mouser.com/ProductDetail/Murata-Electronics/LQW18AN9N1D00D?qs=EPZCdHdMnYJMYfHLXCR5Dg%3D%3D&amp;_gl=1*o1ihxe*_ga*dW5kZWZpbmVk*_ga_15W4STQT4T*dW5kZWZpbmVk*_ga_1KQLCYKRX3*dW5kZWZpbmVk</t>
   </si>
 </sst>
 </file>
@@ -853,7 +853,7 @@
   <dimension ref="A1:K28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -881,7 +881,7 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F1" t="s">
         <v>3</v>
@@ -896,10 +896,10 @@
         <v>25</v>
       </c>
       <c r="J1" s="12" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="K1" s="12" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:11">
@@ -926,12 +926,12 @@
         <v>27</v>
       </c>
       <c r="K2" s="15" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="3" spans="1:11">
       <c r="A3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="12" t="s">
@@ -941,7 +941,7 @@
         <v>7</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="G3">
         <v>1</v>
@@ -954,10 +954,10 @@
         <v>2.64</v>
       </c>
       <c r="J3" s="14" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="K3" s="15" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -968,7 +968,7 @@
         <v>32</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>7</v>
@@ -989,7 +989,7 @@
       </c>
       <c r="J4" s="15"/>
       <c r="K4" s="15" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -1000,7 +1000,7 @@
         <v>32</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>7</v>
@@ -1021,7 +1021,7 @@
       </c>
       <c r="J5" s="15"/>
       <c r="K5" s="15" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -1032,7 +1032,7 @@
         <v>32</v>
       </c>
       <c r="C6" s="24" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>7</v>
@@ -1053,7 +1053,7 @@
       </c>
       <c r="J6" s="15"/>
       <c r="K6" s="15" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -1064,7 +1064,7 @@
         <v>23</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D7" t="s">
         <v>7</v>
@@ -1084,7 +1084,7 @@
       </c>
       <c r="J7" s="14"/>
       <c r="K7" s="15" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -1095,7 +1095,7 @@
         <v>32</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>7</v>
@@ -1116,7 +1116,7 @@
       </c>
       <c r="J8" s="15"/>
       <c r="K8" s="15" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -1127,7 +1127,7 @@
         <v>32</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>7</v>
@@ -1148,7 +1148,7 @@
       </c>
       <c r="J9" s="15"/>
       <c r="K9" s="15" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -1157,10 +1157,10 @@
         <v>36</v>
       </c>
       <c r="C10" s="18" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D10" s="18" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E10" s="5"/>
       <c r="F10" s="12"/>
@@ -1176,25 +1176,25 @@
       </c>
       <c r="J10" s="15"/>
       <c r="K10" s="15" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="11" spans="1:11">
       <c r="A11" s="24" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B11" s="25" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C11" s="24" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D11" s="24" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E11" s="24"/>
       <c r="F11" s="24" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="G11">
         <v>3</v>
@@ -1207,19 +1207,19 @@
         <v>3.4799999999999995</v>
       </c>
       <c r="J11" s="14" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="K11" s="15"/>
     </row>
     <row r="12" spans="1:11">
       <c r="A12" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D12" s="20" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="G12">
         <v>1</v>
@@ -1231,7 +1231,7 @@
       </c>
       <c r="J12" s="15"/>
       <c r="K12" s="15" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="13" spans="1:11">
@@ -1240,7 +1240,7 @@
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="12" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D13" t="s">
         <v>21</v>
@@ -1259,18 +1259,18 @@
         <v>22</v>
       </c>
       <c r="K13" s="15" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="14" spans="1:11">
       <c r="A14" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="G14">
         <v>1</v>
@@ -1283,10 +1283,10 @@
         <v>2.5099999999999998</v>
       </c>
       <c r="J14" s="15" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="K14" s="15" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="15" spans="1:11">
@@ -1316,12 +1316,12 @@
         <v>19</v>
       </c>
       <c r="K15" s="15" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="16" spans="1:11">
       <c r="A16" t="s">
-        <v>42</v>
+        <v>130</v>
       </c>
       <c r="B16" s="8" t="s">
         <v>36</v>
@@ -1340,29 +1340,29 @@
         <v>1</v>
       </c>
       <c r="H16" s="3">
-        <v>0.63</v>
+        <v>0.22</v>
       </c>
       <c r="I16" s="6">
         <f t="shared" ref="I16:I28" si="1">H16*G16</f>
-        <v>0.63</v>
+        <v>0.22</v>
       </c>
       <c r="J16" s="15" t="s">
-        <v>41</v>
+        <v>131</v>
       </c>
       <c r="K16" s="15"/>
     </row>
     <row r="17" spans="1:11">
       <c r="A17" t="s">
+        <v>122</v>
+      </c>
+      <c r="B17" s="27" t="s">
+        <v>43</v>
+      </c>
+      <c r="C17" s="24" t="s">
+        <v>123</v>
+      </c>
+      <c r="D17" t="s">
         <v>124</v>
-      </c>
-      <c r="B17" s="27" t="s">
-        <v>45</v>
-      </c>
-      <c r="C17" s="24" t="s">
-        <v>125</v>
-      </c>
-      <c r="D17" t="s">
-        <v>126</v>
       </c>
       <c r="F17" s="24"/>
       <c r="G17">
@@ -1376,7 +1376,7 @@
         <v>0.36</v>
       </c>
       <c r="J17" s="14" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="K17" s="15"/>
     </row>
@@ -1388,13 +1388,13 @@
         <v>36</v>
       </c>
       <c r="C18" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D18" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="F18" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="G18">
         <v>3</v>
@@ -1417,7 +1417,7 @@
         <v>32</v>
       </c>
       <c r="C19" s="22" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D19" t="s">
         <v>11</v>
@@ -1437,7 +1437,7 @@
       </c>
       <c r="J19" s="15"/>
       <c r="K19" s="15" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="14.25" customHeight="1">
@@ -1448,13 +1448,13 @@
         <v>32</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D20" t="s">
         <v>11</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G20">
         <v>1</v>
@@ -1471,13 +1471,13 @@
     </row>
     <row r="21" spans="1:11">
       <c r="A21" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C21" s="21" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E21" s="5"/>
       <c r="G21">
@@ -1491,28 +1491,28 @@
         <v>0.56000000000000005</v>
       </c>
       <c r="J21" s="17" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="K21" s="15" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="22" spans="1:11">
       <c r="A22" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="B22" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="C22" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="B22" s="12" t="s">
+      <c r="D22" s="12" t="s">
         <v>69</v>
-      </c>
-      <c r="C22" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="D22" s="12" t="s">
-        <v>71</v>
       </c>
       <c r="E22" s="5"/>
       <c r="F22" s="24" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="G22">
         <v>0</v>
@@ -1525,21 +1525,21 @@
         <v>0</v>
       </c>
       <c r="J22" s="17" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="K22" s="15" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="23" spans="1:11">
       <c r="A23" s="5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C23" s="12" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D23" t="s">
         <v>4</v>
@@ -1555,24 +1555,24 @@
         <v>0.8</v>
       </c>
       <c r="J23" s="15" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="K23" s="15" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="24" spans="1:11">
       <c r="A24" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C24" s="12" t="s">
         <v>14</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E24" s="5"/>
       <c r="G24">
@@ -1586,24 +1586,24 @@
         <v>44</v>
       </c>
       <c r="J24" s="15" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="K24" s="15" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="25" spans="1:11">
       <c r="A25" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B25" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C25" s="12" t="s">
         <v>5</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E25" s="5"/>
       <c r="G25">
@@ -1617,10 +1617,10 @@
         <v>1.35</v>
       </c>
       <c r="J25" s="15" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="K25" s="15" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="26" spans="1:11">
@@ -1628,13 +1628,13 @@
         <v>13</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C26" s="12" t="s">
         <v>28</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E26" s="5"/>
       <c r="G26">
@@ -1648,21 +1648,21 @@
         <v>0.47</v>
       </c>
       <c r="J26" s="15" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="27" spans="1:11">
       <c r="A27" s="23" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B27" s="23" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C27" s="24" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D27" s="18" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="G27">
         <v>0</v>
@@ -1675,15 +1675,15 @@
         <v>0</v>
       </c>
       <c r="J27" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="28" spans="1:11">
       <c r="A28" s="22" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D28" s="22" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="G28">
         <v>1</v>
@@ -1696,7 +1696,7 @@
         <v>2.99</v>
       </c>
       <c r="J28" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
   </sheetData>

</xml_diff>